<commit_message>
Fixes duration and assignment of sub-jobs in FullJobShopProblem
</commit_message>
<xml_diff>
--- a/src/examples/data_v1.xlsx
+++ b/src/examples/data_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://datarefineryamsterdam.sharepoint.com/sites/DataRefineryAmsterdam/Gedeelde  documenten/DRA/Projecten/UVA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Documents\Skola\UvA\Y3P6\git_folder\src\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="280" documentId="8_{79064FB8-53C5-496B-B23D-48A92D2D8CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADF73960-F86F-4C2A-A8D9-4B48A5013460}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70BA415A-3E61-4EE7-B169-F68927D11039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="3" xr2:uid="{21867907-8644-4FEF-AD2C-B5CBC4375404}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{21867907-8644-4FEF-AD2C-B5CBC4375404}"/>
   </bookViews>
   <sheets>
     <sheet name="workstations" sheetId="1" r:id="rId1"/>
@@ -271,10 +271,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,6 +293,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -329,18 +335,17 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -690,22 +695,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89040D78-AF12-4A12-A370-EC55FFB56A99}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+      <selection activeCell="A3" sqref="A3:G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -728,7 +733,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -751,7 +756,7 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -775,7 +780,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -798,6 +803,10 @@
       <c r="G4" s="1">
         <v>0.95833333333333337</v>
       </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -809,20 +818,20 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="A5" sqref="A5:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>32</v>
       </c>
@@ -839,7 +848,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -853,7 +862,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -867,43 +876,41 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="8">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8" t="s">
+      <c r="E4" t="s">
         <v>41</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="8">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8" t="s">
+      <c r="E5" t="s">
         <v>41</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -920,7 +927,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -937,7 +944,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -954,7 +961,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -971,7 +978,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -988,7 +995,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1005,7 +1012,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1022,7 +1029,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1039,7 +1046,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1056,7 +1063,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1073,7 +1080,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1090,7 +1097,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1120,16 +1127,16 @@
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>36</v>
       </c>
@@ -1146,7 +1153,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4</v>
       </c>
@@ -1163,7 +1170,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -1180,7 +1187,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6</v>
       </c>
@@ -1197,7 +1204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>7</v>
       </c>
@@ -1214,7 +1221,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>8</v>
       </c>
@@ -1231,7 +1238,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>9</v>
       </c>
@@ -1248,7 +1255,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10</v>
       </c>
@@ -1265,7 +1272,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>11</v>
       </c>
@@ -1282,7 +1289,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>12</v>
       </c>
@@ -1299,7 +1306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>13</v>
       </c>
@@ -1316,7 +1323,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>14</v>
       </c>
@@ -1333,7 +1340,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>15</v>
       </c>
@@ -1358,26 +1365,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC937947-79C6-4845-9815-5221CBDFF226}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D9" sqref="A9:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="22.36328125" customWidth="1"/>
-    <col min="5" max="5" width="64.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" customWidth="1"/>
+    <col min="5" max="5" width="64.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>46</v>
       </c>
@@ -1400,7 +1407,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -1425,7 +1432,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -1450,7 +1457,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -1475,7 +1482,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -1500,7 +1507,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -1525,7 +1532,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -1550,7 +1557,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -1575,13 +1582,128 @@
         <v>720</v>
       </c>
     </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="2"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010029AACF1E989DD642A68A060528E16EE8" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7a178b7e379bfb399d93bd573acf2ee2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1ad5ad67-15a6-48b9-912e-a20f469816cf" xmlns:ns3="ae52d456-94b7-4f7d-986d-6e761dfce4c3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="37de965a0f1fe4956c850926ce0bb72f" ns2:_="" ns3:_="">
     <xsd:import namespace="1ad5ad67-15a6-48b9-912e-a20f469816cf"/>
@@ -1830,15 +1952,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1851,6 +1964,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0F8FD59-1AC4-44F2-B33D-45DC9F9B0863}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B09BE82-5C3B-46BB-A2CE-01AFF08E6431}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1869,14 +1990,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0F8FD59-1AC4-44F2-B33D-45DC9F9B0863}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{173CBD6E-BF29-4475-956A-8CA72BBBB9FC}">
   <ds:schemaRefs>

</xml_diff>